<commit_message>
Plot for part 1 finalized (almost)
</commit_message>
<xml_diff>
--- a/Lab 12/T_SIG_ALL.xlsx
+++ b/Lab 12/T_SIG_ALL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pearl\Desktop\Edumacation\ATSC 303\Lab 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EECE389-6E67-4C6D-A5B8-48BF4BE42F68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ED619D-6A48-46FE-9A89-0FE9A4EFBD33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Time (s)</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Lon (degN)</t>
-  </si>
-  <si>
-    <t>P (kPa)</t>
   </si>
 </sst>
 </file>
@@ -88,24 +85,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,10 +105,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -141,209 +124,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>249660</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>131760</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>271980</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>136800</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="2" name="Ink 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{198B052B-8D91-4F44-A2F5-801568EB3705}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2192760" y="131760"/>
-            <a:ext cx="22320" cy="5040"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="2" name="Ink 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{198B052B-8D91-4F44-A2F5-801568EB3705}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2175120" y="95760"/>
-              <a:ext cx="57960" cy="76680"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>424620</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>446940</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="3" name="Ink 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1B4B7AF-59BD-47ED-8D7B-20838AF9D3AD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="2367720" y="69840"/>
-            <a:ext cx="22320" cy="50040"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="3" name="Ink 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1B4B7AF-59BD-47ED-8D7B-20838AF9D3AD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2350080" y="34200"/>
-              <a:ext cx="57960" cy="121680"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2020-04-10T03:52:49.577"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFC00"/>
-      <inkml:brushProperty name="tip" value="rectangle"/>
-      <inkml:brushProperty name="rasterOp" value="maskPen"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">62 13 9040 0 0,'-15'-7'400'0'0,"6"7"80"0"0,2-3-384 0 0,0 3-96 0 0,-5-3 0 0 0,5 6 0 0 0,7-3 0 0 0,0 0-128 0 0,-4 0 24 0 0,4 0 8 0 0,0 0-72 0 0,0 0-16 0 0,0 0 0 0 0</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
-          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
-          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2020-04-10T03:52:50.540"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.1" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
-      <inkml:brushProperty name="color" value="#FFFC00"/>
-      <inkml:brushProperty name="tip" value="rectangle"/>
-      <inkml:brushProperty name="rasterOp" value="maskPen"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">25 139 5984 0 0,'-1'-4'95'0'0,"1"0"-1"0"0,-1 1 1 0 0,0-1 0 0 0,0 0 0 0 0,-1 1 0 0 0,1-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,-2 0-95 0 0,2 1 144 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,0 0-1 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,1 0-145 0 0,0 2 92 0 0,0 1 0 0 0,0-1 0 0 0,0 0 0 0 0,0 0 0 0 0,0 0 0 0 0,1 0 1 0 0,-1 1-1 0 0,1-1 0 0 0,-1 0 0 0 0,1 0 0 0 0,0 1 0 0 0,0-1 0 0 0,0 1 0 0 0,0-1 1 0 0,0 0-1 0 0,0 1 0 0 0,0 0 0 0 0,0-1 0 0 0,1 0-92 0 0,8-12-30 0 0,-9 12 89 0 0,-2 3 42 0 0,20-16 35 0 0,-12 12-152 0 0,-7 3-1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0-1 0 0,1 0 1 0 0,-1 0 0 0 0,1 0 0 0 0,-1 0 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,-1 1 0 0 0,0-1 0 0 0,1 0-1 0 0,-1 0 1 0 0,1 0 0 0 0,0 1 17 0 0,-1-1-73 0 0,2 1-279 0 0</inkml:trace>
-</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -609,696 +389,636 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A2" sqref="A2:M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.06640625" style="3"/>
+    <col min="2" max="2" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>13</v>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>999.8</v>
       </c>
-      <c r="C2" s="1">
-        <f>(B2*0.001)/0.01</f>
-        <v>99.98</v>
+      <c r="C2">
+        <v>88</v>
       </c>
       <c r="D2">
-        <v>88</v>
-      </c>
-      <c r="E2" s="2">
         <v>6.0500000000000096</v>
       </c>
+      <c r="E2">
+        <v>2.8500000000000201</v>
+      </c>
       <c r="F2">
-        <v>2.8500000000000201</v>
+        <v>80</v>
       </c>
       <c r="G2">
-        <v>80</v>
+        <v>-12.34</v>
       </c>
       <c r="H2">
-        <v>-12.34</v>
+        <v>-0.43</v>
       </c>
       <c r="I2">
-        <v>-0.43</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>12.3</v>
       </c>
       <c r="K2">
-        <v>12.3</v>
+        <v>44.28</v>
       </c>
       <c r="L2">
-        <v>44.28</v>
+        <v>-123.24</v>
       </c>
       <c r="M2">
-        <v>-123.24</v>
-      </c>
-      <c r="N2">
         <v>49.25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>14</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>995.7</v>
       </c>
-      <c r="C3" s="1">
-        <f>(B3*0.001)/0.01</f>
-        <v>99.570000000000007</v>
+      <c r="C3">
+        <v>121</v>
       </c>
       <c r="D3">
-        <v>121</v>
-      </c>
-      <c r="E3" s="2">
         <v>5.0500000000000096</v>
       </c>
+      <c r="E3">
+        <v>-0.75</v>
+      </c>
       <c r="F3">
-        <v>-0.75</v>
+        <v>66</v>
       </c>
       <c r="G3">
-        <v>66</v>
+        <v>2.17</v>
       </c>
       <c r="H3">
-        <v>2.17</v>
+        <v>2.39</v>
       </c>
       <c r="I3">
-        <v>2.39</v>
+        <v>228</v>
       </c>
       <c r="J3">
-        <v>228</v>
+        <v>3.2</v>
       </c>
       <c r="K3">
-        <v>3.2</v>
+        <v>11.52</v>
       </c>
       <c r="L3">
-        <v>11.52</v>
+        <v>-123.24</v>
       </c>
       <c r="M3">
-        <v>-123.24</v>
-      </c>
-      <c r="N3">
         <v>49.25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>138</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>951.8</v>
       </c>
-      <c r="C4" s="1">
-        <f>(B4*0.001)/0.01</f>
-        <v>95.179999999999993</v>
+      <c r="C4">
+        <v>489</v>
       </c>
       <c r="D4">
-        <v>489</v>
-      </c>
-      <c r="E4" s="2">
         <v>3.6500000000000301</v>
       </c>
+      <c r="E4">
+        <v>-2.3499999999999699</v>
+      </c>
       <c r="F4">
-        <v>-2.3499999999999699</v>
+        <v>64</v>
       </c>
       <c r="G4">
-        <v>64</v>
+        <v>-1.21</v>
       </c>
       <c r="H4">
-        <v>-1.21</v>
+        <v>-3.51</v>
       </c>
       <c r="I4">
-        <v>-3.51</v>
+        <v>71</v>
       </c>
       <c r="J4">
-        <v>71</v>
+        <v>3.7</v>
       </c>
       <c r="K4">
-        <v>3.7</v>
+        <v>13.32</v>
       </c>
       <c r="L4">
-        <v>13.32</v>
+        <v>-123.24</v>
       </c>
       <c r="M4">
-        <v>-123.24</v>
-      </c>
-      <c r="N4">
         <v>49.25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>160</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>947</v>
       </c>
-      <c r="C5" s="1">
-        <f>(B5*0.001)/0.01</f>
-        <v>94.7</v>
+      <c r="C5">
+        <v>530</v>
       </c>
       <c r="D5">
-        <v>530</v>
-      </c>
-      <c r="E5" s="2">
         <v>5.1500000000000297</v>
       </c>
+      <c r="E5">
+        <v>-7.25</v>
+      </c>
       <c r="F5">
-        <v>-7.25</v>
+        <v>40</v>
       </c>
       <c r="G5">
-        <v>40</v>
+        <v>-0.99</v>
       </c>
       <c r="H5">
-        <v>-0.99</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="I5">
-        <v>-4.5999999999999996</v>
+        <v>78</v>
       </c>
       <c r="J5">
-        <v>78</v>
+        <v>4.7</v>
       </c>
       <c r="K5">
-        <v>4.7</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="L5">
-        <v>16.920000000000002</v>
+        <v>-123.24</v>
       </c>
       <c r="M5">
-        <v>-123.24</v>
-      </c>
-      <c r="N5">
         <v>49.25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2164</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="2">
         <v>531.20000000000005</v>
       </c>
-      <c r="C6" s="1">
-        <f>(B6*0.001)/0.01</f>
-        <v>53.12</v>
+      <c r="C6">
+        <v>4972</v>
       </c>
       <c r="D6">
-        <v>4972</v>
-      </c>
-      <c r="E6" s="2">
         <v>-27.85</v>
       </c>
+      <c r="E6">
+        <v>-29.95</v>
+      </c>
       <c r="F6">
-        <v>-29.95</v>
+        <v>82</v>
       </c>
       <c r="G6">
-        <v>82</v>
+        <v>7.7</v>
       </c>
       <c r="H6">
-        <v>7.7</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="I6">
-        <v>9.6300000000000008</v>
+        <v>231</v>
       </c>
       <c r="J6">
-        <v>231</v>
+        <v>12.3</v>
       </c>
       <c r="K6">
-        <v>12.3</v>
+        <v>44.28</v>
       </c>
       <c r="L6">
-        <v>44.28</v>
+        <v>-123.25</v>
       </c>
       <c r="M6">
-        <v>-123.25</v>
-      </c>
-      <c r="N6">
         <v>49.37</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2316</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>507.7</v>
       </c>
-      <c r="C7" s="1">
-        <f>(B7*0.001)/0.01</f>
-        <v>50.77</v>
+      <c r="C7">
+        <v>5296</v>
       </c>
       <c r="D7">
-        <v>5296</v>
-      </c>
-      <c r="E7" s="2">
         <v>-27.85</v>
       </c>
+      <c r="E7">
+        <v>-52.35</v>
+      </c>
       <c r="F7">
-        <v>-52.35</v>
+        <v>8</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>4.79</v>
       </c>
       <c r="H7">
-        <v>4.79</v>
+        <v>6.1</v>
       </c>
       <c r="I7">
-        <v>6.1</v>
+        <v>232</v>
       </c>
       <c r="J7">
-        <v>232</v>
+        <v>7.8</v>
       </c>
       <c r="K7">
-        <v>7.8</v>
+        <v>28.08</v>
       </c>
       <c r="L7">
-        <v>28.08</v>
+        <v>-123.24</v>
       </c>
       <c r="M7">
-        <v>-123.24</v>
-      </c>
-      <c r="N7">
         <v>49.38</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>4146</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>276.8</v>
       </c>
-      <c r="C8" s="1">
-        <f>(B8*0.001)/0.01</f>
-        <v>27.68</v>
+      <c r="C8">
+        <v>9379</v>
       </c>
       <c r="D8">
-        <v>9379</v>
-      </c>
-      <c r="E8" s="2">
         <v>-55.25</v>
       </c>
+      <c r="E8">
+        <v>-69.349999999999994</v>
+      </c>
       <c r="F8">
-        <v>-69.349999999999994</v>
+        <v>16</v>
       </c>
       <c r="G8">
-        <v>16</v>
+        <v>9.86</v>
       </c>
       <c r="H8">
-        <v>9.86</v>
+        <v>6.97</v>
       </c>
       <c r="I8">
-        <v>6.97</v>
+        <v>215</v>
       </c>
       <c r="J8">
-        <v>215</v>
+        <v>12.1</v>
       </c>
       <c r="K8">
-        <v>12.1</v>
+        <v>43.56</v>
       </c>
       <c r="L8">
-        <v>43.56</v>
+        <v>-123.13</v>
       </c>
       <c r="M8">
-        <v>-123.13</v>
-      </c>
-      <c r="N8">
         <v>49.51</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>4776</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="2">
         <v>219.8</v>
       </c>
-      <c r="C9" s="1">
-        <f>(B9*0.001)/0.01</f>
-        <v>21.98</v>
+      <c r="C9">
+        <v>10862</v>
       </c>
       <c r="D9">
-        <v>10862</v>
-      </c>
-      <c r="E9" s="2">
         <v>-50.25</v>
       </c>
+      <c r="E9">
+        <v>-82.25</v>
+      </c>
       <c r="F9">
-        <v>-82.25</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>7.2</v>
       </c>
       <c r="H9">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I9">
+        <v>184</v>
+      </c>
+      <c r="J9">
         <v>7.2</v>
       </c>
-      <c r="I9">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="J9">
-        <v>184</v>
-      </c>
       <c r="K9">
-        <v>7.2</v>
+        <v>25.92</v>
       </c>
       <c r="L9">
-        <v>25.92</v>
+        <v>-123.12</v>
       </c>
       <c r="M9">
-        <v>-123.12</v>
-      </c>
-      <c r="N9">
         <v>49.57</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>5778</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="2">
         <v>151.4</v>
       </c>
-      <c r="C10" s="1">
-        <f>(B10*0.001)/0.01</f>
-        <v>15.14</v>
+      <c r="C10">
+        <v>13305</v>
       </c>
       <c r="D10">
-        <v>13305</v>
-      </c>
-      <c r="E10" s="2">
         <v>-48.25</v>
       </c>
+      <c r="E10">
+        <v>-82.55</v>
+      </c>
       <c r="F10">
-        <v>-82.55</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>8.65</v>
       </c>
       <c r="H10">
-        <v>8.65</v>
+        <v>2.73</v>
       </c>
       <c r="I10">
-        <v>2.73</v>
+        <v>198</v>
       </c>
       <c r="J10">
-        <v>198</v>
+        <v>9.1</v>
       </c>
       <c r="K10">
-        <v>9.1</v>
+        <v>32.76</v>
       </c>
       <c r="L10">
-        <v>32.76</v>
+        <v>-123.1</v>
       </c>
       <c r="M10">
-        <v>-123.1</v>
-      </c>
-      <c r="N10">
         <v>49.64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>6178</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>128.69999999999999</v>
       </c>
-      <c r="C11" s="1">
-        <f>(B11*0.001)/0.01</f>
-        <v>12.869999999999997</v>
+      <c r="C11">
+        <v>14366</v>
       </c>
       <c r="D11">
-        <v>14366</v>
-      </c>
-      <c r="E11" s="2">
         <v>-51.65</v>
       </c>
+      <c r="E11">
+        <v>-84.95</v>
+      </c>
       <c r="F11">
-        <v>-84.95</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="H11">
-        <v>8.7100000000000009</v>
+        <v>1.73</v>
       </c>
       <c r="I11">
-        <v>1.73</v>
+        <v>191</v>
       </c>
       <c r="J11">
-        <v>191</v>
+        <v>8.9</v>
       </c>
       <c r="K11">
-        <v>8.9</v>
+        <v>32.04</v>
       </c>
       <c r="L11">
-        <v>32.04</v>
+        <v>-123.09</v>
       </c>
       <c r="M11">
-        <v>-123.09</v>
-      </c>
-      <c r="N11">
         <v>49.66</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>6938</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="2">
         <v>94.8</v>
       </c>
-      <c r="C12" s="1">
-        <f>(B12*0.001)/0.01</f>
-        <v>9.4799999999999986</v>
+      <c r="C12">
+        <v>16355</v>
       </c>
       <c r="D12">
-        <v>16355</v>
-      </c>
-      <c r="E12" s="2">
         <v>-50.35</v>
       </c>
+      <c r="E12">
+        <v>-84.05</v>
+      </c>
       <c r="F12">
-        <v>-84.05</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>10.74</v>
       </c>
       <c r="H12">
-        <v>10.74</v>
+        <v>3.57</v>
       </c>
       <c r="I12">
-        <v>3.57</v>
+        <v>198</v>
       </c>
       <c r="J12">
-        <v>198</v>
+        <v>11.3</v>
       </c>
       <c r="K12">
-        <v>11.3</v>
+        <v>40.68</v>
       </c>
       <c r="L12">
-        <v>40.68</v>
+        <v>-123.06</v>
       </c>
       <c r="M12">
-        <v>-123.06</v>
-      </c>
-      <c r="N12">
         <v>49.71</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>7590</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>72.2</v>
       </c>
-      <c r="C13" s="1">
-        <f>(B13*0.001)/0.01</f>
-        <v>7.22</v>
+      <c r="C13">
+        <v>18115</v>
       </c>
       <c r="D13">
-        <v>18115</v>
-      </c>
-      <c r="E13" s="2">
         <v>-54.45</v>
       </c>
+      <c r="E13">
+        <v>-86.85</v>
+      </c>
       <c r="F13">
-        <v>-86.85</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>6.8</v>
       </c>
       <c r="H13">
-        <v>6.8</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I13">
-        <v>1.1399999999999999</v>
+        <v>190</v>
       </c>
       <c r="J13">
-        <v>190</v>
+        <v>6.9</v>
       </c>
       <c r="K13">
-        <v>6.9</v>
+        <v>24.84</v>
       </c>
       <c r="L13">
-        <v>24.84</v>
+        <v>-123.03</v>
       </c>
       <c r="M13">
-        <v>-123.03</v>
-      </c>
-      <c r="N13">
         <v>49.74</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>8318</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="2">
         <v>53.7</v>
       </c>
-      <c r="C14" s="1">
-        <f>(B14*0.001)/0.01</f>
-        <v>5.37</v>
+      <c r="C14">
+        <v>20027</v>
       </c>
       <c r="D14">
-        <v>20027</v>
-      </c>
-      <c r="E14" s="2">
         <v>-50.05</v>
       </c>
+      <c r="E14">
+        <v>-83.85</v>
+      </c>
       <c r="F14">
-        <v>-83.85</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2.42</v>
       </c>
       <c r="H14">
-        <v>2.42</v>
+        <v>-3.31</v>
       </c>
       <c r="I14">
-        <v>-3.31</v>
+        <v>126</v>
       </c>
       <c r="J14">
-        <v>126</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="K14">
-        <v>4.0999999999999996</v>
+        <v>14.76</v>
       </c>
       <c r="L14">
-        <v>14.76</v>
+        <v>-123.01</v>
       </c>
       <c r="M14">
-        <v>-123.01</v>
-      </c>
-      <c r="N14">
         <v>49.76</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>8584</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>47.9</v>
       </c>
-      <c r="C15" s="1">
-        <f>(B15*0.001)/0.01</f>
-        <v>4.79</v>
+      <c r="C15">
+        <v>20763</v>
       </c>
       <c r="D15">
-        <v>20763</v>
-      </c>
-      <c r="E15" s="2">
         <v>-52.15</v>
       </c>
+      <c r="E15">
+        <v>-85.25</v>
+      </c>
       <c r="F15">
-        <v>-85.25</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>3.25</v>
       </c>
       <c r="H15">
-        <v>3.25</v>
+        <v>-6.21</v>
       </c>
       <c r="I15">
-        <v>-6.21</v>
+        <v>118</v>
       </c>
       <c r="J15">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="K15">
-        <v>7</v>
+        <v>25.2</v>
       </c>
       <c r="L15">
-        <v>25.2</v>
+        <v>-123.02</v>
       </c>
       <c r="M15">
-        <v>-123.02</v>
-      </c>
-      <c r="N15">
         <v>49.76</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N15">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M15">
     <sortCondition descending="1" ref="B2:B15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>